<commit_message>
change in primers names
</commit_message>
<xml_diff>
--- a/qPCR_Analysis.xlsx
+++ b/qPCR_Analysis.xlsx
@@ -158,13 +158,13 @@
     <t xml:space="preserve">Primer</t>
   </si>
   <si>
-    <t xml:space="preserve">Primer1:  GAPDH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Primer2:  3_10860</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Primer3:   6_11180</t>
+    <t xml:space="preserve">Primer_A:  Actin (Pa_2_11200)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primer_B : Pa_5_80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primer3: </t>
   </si>
   <si>
     <t xml:space="preserve">Condition</t>
@@ -288,9 +288,8 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF595959"/>
-      <name val="Calibri"/>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
@@ -752,7 +751,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -798,10 +797,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0566526673219551"/>
-          <c:y val="0.126532567049808"/>
-          <c:w val="0.871727280850684"/>
-          <c:h val="0.717816091954023"/>
+          <c:x val="0.0566425444474225"/>
+          <c:y val="0.126544688188524"/>
+          <c:w val="0.871705530242116"/>
+          <c:h val="0.717789060254814"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -957,11 +956,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="22160016"/>
-        <c:axId val="82961842"/>
+        <c:axId val="59538244"/>
+        <c:axId val="69605769"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="22160016"/>
+        <c:axId val="59538244"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1037,12 +1036,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82961842"/>
+        <c:crossAx val="69605769"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="82961842"/>
+        <c:axId val="69605769"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1088,8 +1087,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.935483870967742"/>
-              <c:y val="0.448275862068966"/>
+              <c:x val="0.935450728133655"/>
+              <c:y val="0.448127215250503"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -1126,7 +1125,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="22160016"/>
+        <c:crossAx val="59538244"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1165,9 +1164,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>471960</xdr:colOff>
+      <xdr:colOff>471600</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>166320</xdr:rowOff>
+      <xdr:rowOff>165960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1175,8 +1174,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="12538080" y="408960"/>
-        <a:ext cx="8057160" cy="3758040"/>
+        <a:off x="12544920" y="408960"/>
+        <a:ext cx="8058600" cy="3757680"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1200,7 +1199,7 @@
       <selection pane="topLeft" activeCell="N3" activeCellId="0" sqref="N3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.78125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.7890625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3.55"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="15" min="2" style="1" width="10.78"/>
@@ -1918,10 +1917,10 @@
   <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
+      <selection pane="topLeft" activeCell="H26" activeCellId="0" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.78125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.7890625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="3.55"/>

</xml_diff>